<commit_message>
started new center base derivation of line of thrust
</commit_message>
<xml_diff>
--- a/docs/input_template_dam2_no_dload.xlsx
+++ b/docs/input_template_dam2_no_dload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E36C95-AE51-3547-81D1-44D1C7F635F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A88C64-F06B-3F4A-B718-7B1EF4982858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9040" yWindow="1340" windowWidth="32920" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
@@ -6111,7 +6111,7 @@
   <dimension ref="B2:P29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>